<commit_message>
Added user search and some styles.
Evaluation protocol should look better now. Aaaand forgot to push... So
there is also a function that prevents guests from going past the
welcome/login/register screen if not logged in.
</commit_message>
<xml_diff>
--- a/08 JS Frameworks/Angular/Social Network/Self-Evaluation-Protocol.xlsx
+++ b/08 JS Frameworks/Angular/Social Network/Self-Evaluation-Protocol.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emil\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emil\Desktop\SoftUni\GitHub\SoftUni\08 JS Frameworks\Angular\Social Network\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -80,6 +80,9 @@
     <t>Comments</t>
   </si>
   <si>
+    <t>∞</t>
+  </si>
+  <si>
     <t>User Register Screen</t>
   </si>
   <si>
@@ -168,19 +171,13 @@
   </si>
   <si>
     <t>Emil Petrov</t>
-  </si>
-  <si>
-    <t>https://goo.gl/gRy9V9</t>
-  </si>
-  <si>
-    <t>yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,14 +207,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -313,11 +302,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -345,9 +333,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -374,12 +359,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -660,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,96 +667,87 @@
       </c>
     </row>
     <row r="3" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="C4" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
+      <c r="C5" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
     </row>
     <row r="6" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="6">
-        <f>IF(E8 ="yes",D8,0)</f>
         <v>50</v>
       </c>
-      <c r="D8" s="12">
-        <v>50</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>49</v>
-      </c>
+      <c r="D8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="13">
-        <f>IF(E9 ="yes",D9,0)</f>
+      <c r="C9" s="6">
         <v>50</v>
       </c>
-      <c r="D9" s="12">
-        <v>50</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>49</v>
-      </c>
+      <c r="D9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B10" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
+      <c r="B10" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="5">
-        <f>IF(E11 ="yes",D11,0)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D11" s="5">
         <v>10</v>
@@ -787,8 +759,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" ref="C12:C34" si="0">IF(E12 ="yes",D12,0)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D12" s="5">
         <v>30</v>
@@ -800,38 +771,31 @@
         <v>4</v>
       </c>
       <c r="C13" s="5">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D13" s="5">
         <v>5</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C14" s="5">
-        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="D14" s="5">
         <v>10</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D15" s="5">
         <v>5</v>
@@ -839,27 +803,23 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="14" t="s">
-        <v>36</v>
+      <c r="B16" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="C16" s="5">
-        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="D16" s="5">
         <v>10</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="14" t="s">
-        <v>37</v>
+      <c r="B17" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="C17" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D17" s="5">
         <v>3</v>
@@ -867,12 +827,11 @@
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="14" t="s">
-        <v>38</v>
+      <c r="B18" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="C18" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D18" s="5">
         <v>7</v>
@@ -880,82 +839,70 @@
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="14" t="s">
-        <v>39</v>
+      <c r="B19" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="C19" s="5">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D19" s="5">
         <v>10</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="14" t="s">
-        <v>40</v>
+      <c r="B20" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C20" s="5">
-        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D20" s="5">
+        <v>5</v>
+      </c>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="5">
+        <v>10</v>
+      </c>
+      <c r="D21" s="5">
+        <v>10</v>
+      </c>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="5">
         <v>0</v>
       </c>
-      <c r="D20" s="5">
-        <v>5</v>
-      </c>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="5">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="D21" s="5">
-        <v>10</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="D22" s="5">
         <v>10</v>
       </c>
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="14" t="s">
-        <v>43</v>
+      <c r="B23" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="C23" s="5">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D23" s="5">
         <v>5</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="E23" s="5"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="14" t="s">
-        <v>44</v>
+      <c r="B24" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="C24" s="5">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D24" s="5">
@@ -965,27 +912,21 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C25" s="5">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D25" s="5">
         <v>10</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="E25" s="5"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="B26" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="5"/>
       <c r="D26" s="5">
         <v>10</v>
       </c>
@@ -993,10 +934,9 @@
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C27" s="5">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D27" s="5">
@@ -1006,56 +946,46 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C28" s="5">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D28" s="5">
         <v>5</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="E28" s="5"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C29" s="5">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D29" s="5">
         <v>5</v>
       </c>
-      <c r="E29" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="E29" s="5"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C30" s="5">
-        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="D30" s="5">
         <v>10</v>
       </c>
-      <c r="E30" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="E30" s="5"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C31" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D31" s="5">
         <v>5</v>
@@ -1067,23 +997,19 @@
         <v>7</v>
       </c>
       <c r="C32" s="5">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D32" s="5">
         <v>5</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="E32" s="5"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C33" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D33" s="5">
         <v>5</v>
@@ -1092,11 +1018,10 @@
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C34" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D34" s="5">
         <v>10</v>
@@ -1104,62 +1029,50 @@
       <c r="E34" s="5"/>
     </row>
     <row r="35" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B35" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="19"/>
+      <c r="B35" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="18"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" s="7">
-        <f>IF(E36 ="yes",D36,0)</f>
-        <v>0</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C36" s="7"/>
       <c r="D36" s="7">
         <v>10</v>
       </c>
       <c r="E36" s="7"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B37" s="15" t="s">
-        <v>28</v>
+      <c r="B37" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="C37" s="7">
-        <f t="shared" ref="C37:C43" si="1">IF(E37 ="yes",D37,0)</f>
         <v>5</v>
       </c>
       <c r="D37" s="7">
         <v>5</v>
       </c>
-      <c r="E37" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="E37" s="7"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C38" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C38" s="7"/>
       <c r="D38" s="7">
         <v>10</v>
       </c>
       <c r="E38" s="7"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B39" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="B39" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="7"/>
       <c r="D39" s="7">
         <v>5</v>
       </c>
@@ -1167,55 +1080,45 @@
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C40" s="7">
-        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="D40" s="7">
         <v>5</v>
       </c>
-      <c r="E40" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="E40" s="7"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C41" s="7">
-        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="D41" s="7">
         <v>5</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="E41" s="7"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C42" s="7">
-        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="D42" s="7">
         <v>20</v>
       </c>
-      <c r="E42" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="E42" s="7"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B43" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C43" s="7">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D43" s="7">
@@ -1229,7 +1132,7 @@
       </c>
       <c r="C44" s="11">
         <f>SUM(C6:C43)</f>
-        <v>220</v>
+        <v>283</v>
       </c>
       <c r="D44" s="11">
         <v>370</v>
@@ -1246,10 +1149,7 @@
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="C7:E7"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C7" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Some fixes and style fixes and more fixes...
Also you can spam people's walls with posts now!
</commit_message>
<xml_diff>
--- a/08 JS Frameworks/Angular/Social Network/Self-Evaluation-Protocol.xlsx
+++ b/08 JS Frameworks/Angular/Social Network/Self-Evaluation-Protocol.xlsx
@@ -641,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -843,7 +843,7 @@
         <v>40</v>
       </c>
       <c r="C19" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D19" s="5">
         <v>10</v>
@@ -926,7 +926,9 @@
       <c r="B26" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="5"/>
+      <c r="C26" s="5">
+        <v>10</v>
+      </c>
       <c r="D26" s="5">
         <v>10</v>
       </c>
@@ -1132,7 +1134,7 @@
       </c>
       <c r="C44" s="11">
         <f>SUM(C6:C43)</f>
-        <v>299</v>
+        <v>310</v>
       </c>
       <c r="D44" s="11">
         <v>370</v>

</xml_diff>

<commit_message>
Added dynamic scrolling, and notes and things.
</commit_message>
<xml_diff>
--- a/08 JS Frameworks/Angular/Social Network/Self-Evaluation-Protocol.xlsx
+++ b/08 JS Frameworks/Angular/Social Network/Self-Evaluation-Protocol.xlsx
@@ -641,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -650,6 +650,7 @@
     <col min="2" max="2" width="35.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12.5546875" style="9" customWidth="1"/>
     <col min="5" max="5" width="48.6640625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="18" x14ac:dyDescent="0.35">
@@ -747,7 +748,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="5">
         <v>10</v>
@@ -902,9 +903,7 @@
       <c r="B24" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="5">
-        <v>0</v>
-      </c>
+      <c r="C24" s="5"/>
       <c r="D24" s="5">
         <v>5</v>
       </c>
@@ -915,7 +914,7 @@
         <v>20</v>
       </c>
       <c r="C25" s="5">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D25" s="5">
         <v>10</v>
@@ -939,7 +938,7 @@
         <v>21</v>
       </c>
       <c r="C27" s="5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D27" s="5">
         <v>10</v>
@@ -1042,7 +1041,9 @@
       <c r="B36" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="7"/>
+      <c r="C36" s="7">
+        <v>8</v>
+      </c>
       <c r="D36" s="7">
         <v>10</v>
       </c>
@@ -1064,7 +1065,9 @@
       <c r="B38" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C38" s="7"/>
+      <c r="C38" s="7">
+        <v>8</v>
+      </c>
       <c r="D38" s="7">
         <v>10</v>
       </c>
@@ -1074,7 +1077,9 @@
       <c r="B39" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="7"/>
+      <c r="C39" s="7">
+        <v>5</v>
+      </c>
       <c r="D39" s="7">
         <v>5</v>
       </c>
@@ -1134,7 +1139,7 @@
       </c>
       <c r="C44" s="11">
         <f>SUM(C6:C43)</f>
-        <v>310</v>
+        <v>344</v>
       </c>
       <c r="D44" s="11">
         <v>370</v>

</xml_diff>

<commit_message>
Some style changed and logic fixes.
</commit_message>
<xml_diff>
--- a/08 JS Frameworks/Angular/Social Network/Self-Evaluation-Protocol.xlsx
+++ b/08 JS Frameworks/Angular/Social Network/Self-Evaluation-Protocol.xlsx
@@ -641,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>